<commit_message>
Run 1 in the table
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,36 +8,91 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://relexsolutions-my.sharepoint.com/personal/aleksandra_petrenko_relexsolutions_com/Documents/Desktop/WiSe23-24/Masterarbeit Specimen Delivery/Computational experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC1048B7115F539E5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{981A3BD8-627C-4084-B5FE-C3464E6A879F}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="11_F25DC773A252ABDACC1048B7115F539E5ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B28AC8A5-384D-4513-B5CA-DF8360F7FFAF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Passau" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Gap</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Det</t>
+  </si>
+  <si>
+    <t>Prob</t>
+  </si>
+  <si>
+    <t>ProbRel</t>
+  </si>
+  <si>
+    <t>DetRel</t>
+  </si>
+  <si>
+    <t>Price of uncertainty</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,14 +115,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -345,92 +434,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="16.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="8.7265625" style="14"/>
+    <col min="6" max="6" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" style="4"/>
+    <col min="12" max="12" width="8.7265625" style="14"/>
+    <col min="13" max="13" width="12.7265625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1020</v>
-      </c>
-      <c r="B2">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>5100</v>
       </c>
       <c r="B3">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="3"/>
+      <c r="I3" s="3">
+        <f>F3-C3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <f>J3-N3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10200</v>
+        <v>5100</v>
       </c>
       <c r="B4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I11" si="0">F4-C4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M11" si="1">J4-N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>10200</v>
+      </c>
+      <c r="B5">
+        <v>0.97</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>1020</v>
-      </c>
-      <c r="B5">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5100</v>
       </c>
       <c r="B6">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>10200</v>
+        <v>5100</v>
       </c>
       <c r="B7">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>10200</v>
+      </c>
+      <c r="B8">
+        <v>0.98</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>1020</v>
-      </c>
-      <c r="B8">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>5100</v>
       </c>
       <c r="B9">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>10200</v>
+        <v>5100</v>
       </c>
       <c r="B10">
         <v>0.999</v>
       </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10200</v>
+      </c>
+      <c r="B11">
+        <v>0.999</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>